<commit_message>
floyd with edges done, must be debuged to fix rows and columns bug when searching on the edge floyd matrix
</commit_message>
<xml_diff>
--- a/data/Lista lugares.xlsx
+++ b/data/Lista lugares.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\eclipse-workspace\economic-travel\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D560719-1E8D-446D-BC5A-E593DBCA3C65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239BCD99-5355-46E6-89EE-B566115DDF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>Unidad Deportiva Panamericana</t>
   </si>
   <si>
-    <t>Estadio Olimpio Pascual Guerrero</t>
-  </si>
-  <si>
     <t>Gobernacion del Valle</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>Centro comercial Jardin Plaza</t>
+  </si>
+  <si>
+    <t>Estadio Olimpico Pascual Guerrero</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
   <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,7 +561,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -569,7 +569,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -577,7 +577,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -585,7 +585,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -593,7 +593,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -601,7 +601,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -609,7 +609,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -617,7 +617,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -625,7 +625,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -633,7 +633,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -641,7 +641,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -649,7 +649,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -657,7 +657,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -665,7 +665,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -673,7 +673,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -681,7 +681,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -689,7 +689,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -697,7 +697,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -705,7 +705,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -713,7 +713,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -721,7 +721,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -729,7 +729,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -737,7 +737,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -745,7 +745,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -753,7 +753,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -761,7 +761,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -769,7 +769,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -777,7 +777,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -785,7 +785,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -793,7 +793,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -801,7 +801,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -809,7 +809,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>